<commit_message>
Edited some rows of time sheet.
</commit_message>
<xml_diff>
--- a/Week 9- Time Sheet/Sudip-Time Sheet (w-9).xlsx
+++ b/Week 9- Time Sheet/Sudip-Time Sheet (w-9).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heysu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heysu\Documents\My-salon\Week 9- Time Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8736BFB-4A44-4491-BAA1-5489747A5CC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFEEE7B-0B00-42AE-B301-3D591BEFE1F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Hour 1</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>Week 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worked on redirecting non-logged in user to login page when click on Appointment tab </t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -538,10 +541,16 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>